<commit_message>
ajustes tras ejecutar check
</commit_message>
<xml_diff>
--- a/analisisDescriptivo_temp.xlsx
+++ b/analisisDescriptivo_temp.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t xml:space="preserve">Titulo Principal 1</t>
   </si>
@@ -84,10 +84,13 @@
     <t xml:space="preserve">26,7</t>
   </si>
   <si>
-    <t xml:space="preserve">28,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,0</t>
+    <t xml:space="preserve">27,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,1</t>
   </si>
   <si>
     <t xml:space="preserve">21,4</t>
@@ -108,7 +111,7 @@
     <t xml:space="preserve">4,5</t>
   </si>
   <si>
-    <t xml:space="preserve">3,4</t>
+    <t xml:space="preserve">4,7</t>
   </si>
   <si>
     <t xml:space="preserve">▇▂▂▂▁▃▁▃</t>
@@ -120,19 +123,19 @@
     <t xml:space="preserve">19,7</t>
   </si>
   <si>
-    <t xml:space="preserve">19,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-8,8</t>
+    <t xml:space="preserve">18,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-9,7</t>
   </si>
   <si>
     <t xml:space="preserve">0,0000</t>
   </si>
   <si>
-    <t xml:space="preserve">18,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21,1</t>
+    <t xml:space="preserve">15,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20,6</t>
   </si>
   <si>
     <t xml:space="preserve">17,8</t>
@@ -147,7 +150,7 @@
     <t xml:space="preserve">1,5</t>
   </si>
   <si>
-    <t xml:space="preserve">1,4</t>
+    <t xml:space="preserve">0,8</t>
   </si>
   <si>
     <t xml:space="preserve">▅▁▁▂▂▁▁▇</t>
@@ -159,16 +162,16 @@
     <t xml:space="preserve">15,1</t>
   </si>
   <si>
-    <t xml:space="preserve">14,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-14,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16,0</t>
+    <t xml:space="preserve">15,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16,3</t>
   </si>
   <si>
     <t xml:space="preserve">10,4</t>
@@ -177,9 +180,6 @@
     <t xml:space="preserve">14,4</t>
   </si>
   <si>
-    <t xml:space="preserve">15,2</t>
-  </si>
-  <si>
     <t xml:space="preserve">16,2</t>
   </si>
   <si>
@@ -189,7 +189,7 @@
     <t xml:space="preserve">2,6</t>
   </si>
   <si>
-    <t xml:space="preserve">2,7</t>
+    <t xml:space="preserve">1,9</t>
   </si>
   <si>
     <t xml:space="preserve">▃▁▂▃▇▂▂▃</t>
@@ -240,10 +240,10 @@
     <t xml:space="preserve">100,0%</t>
   </si>
   <si>
-    <t xml:space="preserve">14,5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37,0%</t>
+    <t xml:space="preserve">5,9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,4%</t>
   </si>
   <si>
     <t xml:space="preserve">9,1%</t>
@@ -252,22 +252,19 @@
     <t xml:space="preserve">42,9%</t>
   </si>
   <si>
-    <t xml:space="preserve">15,52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,0004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,70</t>
+    <t xml:space="preserve">28,50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,94</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">85,5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63,0%</t>
+    <t xml:space="preserve">94,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90,6%</t>
   </si>
   <si>
     <t xml:space="preserve">90,9%</t>
@@ -754,39 +751,39 @@
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
@@ -798,51 +795,51 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" t="s">
         <v>35</v>
       </c>
-      <c r="H6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" t="s">
-        <v>34</v>
-      </c>
       <c r="O6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -854,31 +851,31 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" t="s">
         <v>49</v>
-      </c>
-      <c r="I7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K7" t="s">
-        <v>51</v>
-      </c>
-      <c r="L7" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" t="s">
-        <v>54</v>
       </c>
       <c r="O7" t="s">
         <v>55</v>
@@ -978,13 +975,13 @@
         <v>76</v>
       </c>
       <c r="F5" t="n">
-        <v>13.7</v>
+        <v>78.7</v>
       </c>
       <c r="G5" t="n">
-        <v>2.3</v>
+        <v>1.3</v>
       </c>
       <c r="H5" t="n">
-        <v>6.5</v>
+        <v>1.8</v>
       </c>
       <c r="I5" t="s">
         <v>74</v>
@@ -999,36 +996,36 @@
         <v>79</v>
       </c>
       <c r="M5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" t="s">
         <v>80</v>
-      </c>
-      <c r="N5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" t="s">
         <v>83</v>
-      </c>
-      <c r="E6" t="s">
-        <v>84</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>13.4</v>
+        <v>21.2</v>
       </c>
       <c r="H6" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I6"/>
       <c r="J6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" t="s">
         <v>85</v>
-      </c>
-      <c r="K6" t="s">
-        <v>86</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>

</xml_diff>